<commit_message>
Street Map pdfs angepasst
</commit_message>
<xml_diff>
--- a/other/Street Map/streets crossings capacities traffic.xlsx
+++ b/other/Street Map/streets crossings capacities traffic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ist-Zustand" sheetId="1" r:id="rId1"/>
@@ -661,22 +661,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.21875" customWidth="1"/>
-    <col min="3" max="3" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
-    <col min="5" max="5" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="38.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>44</v>
       </c>
@@ -688,7 +691,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -705,7 +708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -716,7 +719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
@@ -727,7 +730,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -738,7 +741,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
@@ -749,7 +752,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
@@ -760,7 +763,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
@@ -771,7 +774,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
@@ -782,7 +785,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
@@ -793,7 +796,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>41</v>
       </c>
@@ -804,7 +807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -821,7 +824,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>32</v>
       </c>
@@ -835,7 +838,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>34</v>
       </c>
@@ -849,7 +852,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -866,7 +869,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>25</v>
       </c>
@@ -883,7 +886,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>26</v>
       </c>
@@ -900,7 +903,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>27</v>
       </c>
@@ -917,7 +920,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>28</v>
       </c>
@@ -931,7 +934,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>30</v>
       </c>
@@ -945,7 +948,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>35</v>
       </c>
@@ -959,7 +962,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>36</v>
       </c>
@@ -973,7 +976,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
@@ -987,7 +990,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>38</v>
       </c>
@@ -1001,7 +1004,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>39</v>
       </c>
@@ -1020,22 +1023,25 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="58" orientation="portrait" horizontalDpi="4294967295" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection sqref="A1:M55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>45</v>
       </c>
@@ -1051,7 +1057,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1068,7 +1074,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1079,7 +1085,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1090,7 +1096,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
@@ -1101,7 +1107,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1112,7 +1118,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1123,7 +1129,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
@@ -1134,7 +1140,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
@@ -1145,7 +1151,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
@@ -1156,7 +1162,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>41</v>
       </c>
@@ -1167,7 +1173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -1184,7 +1190,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
@@ -1198,7 +1204,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
@@ -1212,7 +1218,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
@@ -1226,7 +1232,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>43</v>
       </c>
@@ -1240,7 +1246,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>27</v>
       </c>
@@ -1254,7 +1260,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>28</v>
       </c>
@@ -1268,7 +1274,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>35</v>
       </c>
@@ -1282,7 +1288,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>36</v>
       </c>
@@ -1296,7 +1302,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>37</v>
       </c>
@@ -1310,7 +1316,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>38</v>
       </c>
@@ -1324,7 +1330,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>39</v>
       </c>
@@ -1343,7 +1349,7 @@
     <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="59" orientation="portrait" horizontalDpi="4294967295" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>